<commit_message>
calendario + guardar nombre quiz
</commit_message>
<xml_diff>
--- a/tfg/logs_Paula.xlsx
+++ b/tfg/logs_Paula.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e33f79c92a0135/Escritorio/tfg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61e33f79c92a0135/Escritorio/GitHub/TFG/tfg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="8_{95E75934-1E81-49D5-A8E5-797E35BB54EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26E7C1BB-3B7D-4D6B-8258-74962F17B88A}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="8_{95E75934-1E81-49D5-A8E5-797E35BB54EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{655C0C35-9037-4BF1-A7A0-7A483C15AC2D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{48885DB5-F153-4EEB-9C29-0F7AED7AFDA1}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{48885DB5-F153-4EEB-9C29-0F7AED7AFDA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1849,24 +1849,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2980D243-12F6-47ED-9CB5-E7C7CE140448}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I454"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
-    <col min="6" max="6" width="33.88671875" customWidth="1"/>
-    <col min="7" max="7" width="66.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1"/>
+    <col min="7" max="7" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>468</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1953,7 +1952,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2040,7 +2039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2069,7 +2068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2098,7 +2097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2185,7 +2184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2272,7 +2271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2301,7 +2300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2417,7 +2416,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2504,7 +2503,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +2532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2678,7 +2677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2707,7 +2706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2736,7 +2735,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -2968,7 +2967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -3142,7 +3141,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -3171,7 +3170,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -3229,7 +3228,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>78</v>
       </c>
@@ -3258,7 +3257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -3345,7 +3344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -3374,7 +3373,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>83</v>
       </c>
@@ -3403,7 +3402,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -3432,7 +3431,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -3461,7 +3460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -3490,7 +3489,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -3519,7 +3518,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -3577,7 +3576,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>90</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -3693,7 +3692,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -3722,7 +3721,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>90</v>
       </c>
@@ -3751,7 +3750,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>90</v>
       </c>
@@ -3780,7 +3779,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -3838,7 +3837,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>98</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>98</v>
       </c>
@@ -3896,7 +3895,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -3925,7 +3924,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>98</v>
       </c>
@@ -3954,7 +3953,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>98</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>98</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>98</v>
       </c>
@@ -4041,7 +4040,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>104</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
@@ -4099,7 +4098,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>104</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>104</v>
       </c>
@@ -4157,7 +4156,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>104</v>
       </c>
@@ -4186,7 +4185,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>108</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>108</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>109</v>
       </c>
@@ -4273,7 +4272,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>109</v>
       </c>
@@ -4302,7 +4301,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -4331,7 +4330,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>109</v>
       </c>
@@ -4360,7 +4359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>110</v>
       </c>
@@ -4389,7 +4388,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>110</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>110</v>
       </c>
@@ -4447,7 +4446,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>110</v>
       </c>
@@ -4476,7 +4475,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>110</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>110</v>
       </c>
@@ -4534,7 +4533,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>110</v>
       </c>
@@ -4563,7 +4562,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>110</v>
       </c>
@@ -4592,7 +4591,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -4621,7 +4620,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>110</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -4708,7 +4707,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>110</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>110</v>
       </c>
@@ -4766,7 +4765,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -4795,7 +4794,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -4824,7 +4823,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>131</v>
       </c>
@@ -4853,7 +4852,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>132</v>
       </c>
@@ -4882,7 +4881,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>132</v>
       </c>
@@ -4911,7 +4910,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>135</v>
       </c>
@@ -4940,7 +4939,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>135</v>
       </c>
@@ -4969,7 +4968,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>135</v>
       </c>
@@ -4998,7 +4997,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>135</v>
       </c>
@@ -5027,7 +5026,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>140</v>
       </c>
@@ -5056,7 +5055,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>140</v>
       </c>
@@ -5085,7 +5084,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>140</v>
       </c>
@@ -5114,7 +5113,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>142</v>
       </c>
@@ -5143,7 +5142,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>142</v>
       </c>
@@ -5172,7 +5171,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>143</v>
       </c>
@@ -5201,7 +5200,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>145</v>
       </c>
@@ -5230,7 +5229,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>146</v>
       </c>
@@ -5259,7 +5258,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>146</v>
       </c>
@@ -5288,7 +5287,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>150</v>
       </c>
@@ -5317,7 +5316,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>150</v>
       </c>
@@ -5346,7 +5345,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>156</v>
       </c>
@@ -5375,7 +5374,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>159</v>
       </c>
@@ -5404,7 +5403,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>160</v>
       </c>
@@ -5433,7 +5432,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>165</v>
       </c>
@@ -5462,7 +5461,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>166</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="280.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>166</v>
       </c>
@@ -5520,7 +5519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>172</v>
       </c>
@@ -5549,7 +5548,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>172</v>
       </c>
@@ -5578,7 +5577,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>173</v>
       </c>
@@ -5607,7 +5606,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>173</v>
       </c>
@@ -5636,7 +5635,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>173</v>
       </c>
@@ -5665,7 +5664,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>178</v>
       </c>
@@ -5694,7 +5693,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>178</v>
       </c>
@@ -5723,7 +5722,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>182</v>
       </c>
@@ -5752,7 +5751,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>182</v>
       </c>
@@ -5781,7 +5780,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>182</v>
       </c>
@@ -5810,7 +5809,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>184</v>
       </c>
@@ -5839,7 +5838,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>184</v>
       </c>
@@ -5868,7 +5867,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>185</v>
       </c>
@@ -5897,7 +5896,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>186</v>
       </c>
@@ -5926,7 +5925,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>186</v>
       </c>
@@ -5955,7 +5954,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>186</v>
       </c>
@@ -5984,7 +5983,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>190</v>
       </c>
@@ -6013,7 +6012,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>190</v>
       </c>
@@ -6042,7 +6041,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>190</v>
       </c>
@@ -6071,7 +6070,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>190</v>
       </c>
@@ -6100,7 +6099,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>192</v>
       </c>
@@ -6129,7 +6128,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>192</v>
       </c>
@@ -6158,7 +6157,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>192</v>
       </c>
@@ -6187,7 +6186,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>192</v>
       </c>
@@ -6216,7 +6215,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>196</v>
       </c>
@@ -6245,7 +6244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>196</v>
       </c>
@@ -6274,7 +6273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>199</v>
       </c>
@@ -6303,7 +6302,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>199</v>
       </c>
@@ -6332,7 +6331,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>199</v>
       </c>
@@ -6361,7 +6360,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>199</v>
       </c>
@@ -6390,7 +6389,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>199</v>
       </c>
@@ -6419,7 +6418,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>199</v>
       </c>
@@ -6448,7 +6447,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>199</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>199</v>
       </c>
@@ -6506,7 +6505,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>199</v>
       </c>
@@ -6535,7 +6534,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>209</v>
       </c>
@@ -6564,7 +6563,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>210</v>
       </c>
@@ -6593,7 +6592,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>210</v>
       </c>
@@ -6622,7 +6621,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>212</v>
       </c>
@@ -6651,7 +6650,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>212</v>
       </c>
@@ -6680,7 +6679,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>213</v>
       </c>
@@ -6709,7 +6708,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>213</v>
       </c>
@@ -6738,7 +6737,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>213</v>
       </c>
@@ -6767,7 +6766,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>217</v>
       </c>
@@ -6796,7 +6795,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>218</v>
       </c>
@@ -6825,7 +6824,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>218</v>
       </c>
@@ -6854,7 +6853,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>220</v>
       </c>
@@ -6883,7 +6882,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>220</v>
       </c>
@@ -6912,7 +6911,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>221</v>
       </c>
@@ -6941,7 +6940,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>222</v>
       </c>
@@ -6970,7 +6969,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>223</v>
       </c>
@@ -6999,7 +6998,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>223</v>
       </c>
@@ -7028,7 +7027,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>223</v>
       </c>
@@ -7057,7 +7056,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>223</v>
       </c>
@@ -7086,7 +7085,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>223</v>
       </c>
@@ -7115,7 +7114,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>223</v>
       </c>
@@ -7144,7 +7143,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>223</v>
       </c>
@@ -7173,7 +7172,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>223</v>
       </c>
@@ -7202,7 +7201,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>228</v>
       </c>
@@ -7231,7 +7230,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>229</v>
       </c>
@@ -7260,7 +7259,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>229</v>
       </c>
@@ -7289,7 +7288,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>231</v>
       </c>
@@ -7318,7 +7317,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>231</v>
       </c>
@@ -7347,7 +7346,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>231</v>
       </c>
@@ -7376,7 +7375,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>231</v>
       </c>
@@ -7405,7 +7404,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>235</v>
       </c>
@@ -7434,7 +7433,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>235</v>
       </c>
@@ -7463,7 +7462,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>235</v>
       </c>
@@ -7492,7 +7491,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>235</v>
       </c>
@@ -7521,7 +7520,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>239</v>
       </c>
@@ -7550,7 +7549,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>240</v>
       </c>
@@ -7579,7 +7578,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>240</v>
       </c>
@@ -7608,7 +7607,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>240</v>
       </c>
@@ -7637,7 +7636,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>245</v>
       </c>
@@ -7666,7 +7665,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>246</v>
       </c>
@@ -7695,7 +7694,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>247</v>
       </c>
@@ -7724,7 +7723,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>247</v>
       </c>
@@ -7753,7 +7752,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>247</v>
       </c>
@@ -7782,7 +7781,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>250</v>
       </c>
@@ -7811,7 +7810,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>251</v>
       </c>
@@ -7840,7 +7839,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>251</v>
       </c>
@@ -7869,7 +7868,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>251</v>
       </c>
@@ -7898,7 +7897,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>251</v>
       </c>
@@ -7927,7 +7926,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>251</v>
       </c>
@@ -7956,7 +7955,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>251</v>
       </c>
@@ -7985,7 +7984,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>251</v>
       </c>
@@ -8014,7 +8013,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>251</v>
       </c>
@@ -8043,7 +8042,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>256</v>
       </c>
@@ -8072,7 +8071,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>256</v>
       </c>
@@ -8101,7 +8100,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>256</v>
       </c>
@@ -8130,7 +8129,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>256</v>
       </c>
@@ -8159,7 +8158,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>258</v>
       </c>
@@ -8188,7 +8187,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>258</v>
       </c>
@@ -8217,7 +8216,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>263</v>
       </c>
@@ -8246,7 +8245,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>263</v>
       </c>
@@ -8275,7 +8274,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>264</v>
       </c>
@@ -8304,7 +8303,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>264</v>
       </c>
@@ -8333,7 +8332,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>264</v>
       </c>
@@ -8362,7 +8361,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>264</v>
       </c>
@@ -8391,7 +8390,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>264</v>
       </c>
@@ -8420,7 +8419,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>264</v>
       </c>
@@ -8449,7 +8448,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>264</v>
       </c>
@@ -8478,7 +8477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>264</v>
       </c>
@@ -8507,7 +8506,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>264</v>
       </c>
@@ -8536,7 +8535,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>264</v>
       </c>
@@ -8565,7 +8564,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>272</v>
       </c>
@@ -8594,7 +8593,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>272</v>
       </c>
@@ -8623,7 +8622,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>272</v>
       </c>
@@ -8652,7 +8651,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>272</v>
       </c>
@@ -8681,7 +8680,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>274</v>
       </c>
@@ -8710,7 +8709,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>274</v>
       </c>
@@ -8739,7 +8738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="238" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>274</v>
       </c>
@@ -8768,7 +8767,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>274</v>
       </c>
@@ -8797,7 +8796,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>275</v>
       </c>
@@ -8826,7 +8825,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>275</v>
       </c>
@@ -8855,7 +8854,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>276</v>
       </c>
@@ -8884,7 +8883,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>276</v>
       </c>
@@ -8913,7 +8912,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>280</v>
       </c>
@@ -8942,7 +8941,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>280</v>
       </c>
@@ -8971,7 +8970,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>283</v>
       </c>
@@ -9000,7 +8999,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>283</v>
       </c>
@@ -9029,7 +9028,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>283</v>
       </c>
@@ -9058,7 +9057,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>285</v>
       </c>
@@ -9087,7 +9086,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>286</v>
       </c>
@@ -9116,7 +9115,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>286</v>
       </c>
@@ -9145,7 +9144,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>289</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>292</v>
       </c>
@@ -9203,7 +9202,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>293</v>
       </c>
@@ -9232,7 +9231,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>293</v>
       </c>
@@ -9261,7 +9260,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>293</v>
       </c>
@@ -9290,7 +9289,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>297</v>
       </c>
@@ -9319,7 +9318,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>298</v>
       </c>
@@ -9348,7 +9347,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>301</v>
       </c>
@@ -9377,7 +9376,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>302</v>
       </c>
@@ -9406,7 +9405,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>303</v>
       </c>
@@ -9435,7 +9434,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>306</v>
       </c>
@@ -9464,7 +9463,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>306</v>
       </c>
@@ -9493,7 +9492,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>309</v>
       </c>
@@ -9522,7 +9521,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>309</v>
       </c>
@@ -9551,7 +9550,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>312</v>
       </c>
@@ -9580,7 +9579,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>315</v>
       </c>
@@ -9609,7 +9608,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>315</v>
       </c>
@@ -9638,7 +9637,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>315</v>
       </c>
@@ -9667,7 +9666,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>315</v>
       </c>
@@ -9696,7 +9695,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>317</v>
       </c>
@@ -9725,7 +9724,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>317</v>
       </c>
@@ -9754,7 +9753,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>317</v>
       </c>
@@ -9783,7 +9782,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>317</v>
       </c>
@@ -9812,7 +9811,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>317</v>
       </c>
@@ -9841,7 +9840,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>317</v>
       </c>
@@ -9870,7 +9869,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="277" spans="1:9" ht="280.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>317</v>
       </c>
@@ -9899,7 +9898,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>317</v>
       </c>
@@ -9928,7 +9927,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>324</v>
       </c>
@@ -9957,7 +9956,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>324</v>
       </c>
@@ -9986,7 +9985,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>324</v>
       </c>
@@ -10015,7 +10014,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>325</v>
       </c>
@@ -10044,7 +10043,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>325</v>
       </c>
@@ -10073,7 +10072,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>325</v>
       </c>
@@ -10102,7 +10101,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>325</v>
       </c>
@@ -10131,7 +10130,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>329</v>
       </c>
@@ -10160,7 +10159,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>329</v>
       </c>
@@ -10189,7 +10188,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>329</v>
       </c>
@@ -10218,7 +10217,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>332</v>
       </c>
@@ -10247,7 +10246,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>332</v>
       </c>
@@ -10276,7 +10275,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="291" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>332</v>
       </c>
@@ -10305,7 +10304,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="292" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>332</v>
       </c>
@@ -10334,7 +10333,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="293" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>332</v>
       </c>
@@ -10363,7 +10362,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="294" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>332</v>
       </c>
@@ -10392,7 +10391,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="295" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>332</v>
       </c>
@@ -10421,7 +10420,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="296" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>332</v>
       </c>
@@ -10450,7 +10449,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>332</v>
       </c>
@@ -10479,7 +10478,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>332</v>
       </c>
@@ -10508,7 +10507,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>332</v>
       </c>
@@ -10537,7 +10536,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>332</v>
       </c>
@@ -10566,7 +10565,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="301" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>332</v>
       </c>
@@ -10595,7 +10594,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="302" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>332</v>
       </c>
@@ -10624,7 +10623,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="303" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>332</v>
       </c>
@@ -10653,7 +10652,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>332</v>
       </c>
@@ -10682,7 +10681,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>340</v>
       </c>
@@ -10711,7 +10710,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>340</v>
       </c>
@@ -10740,7 +10739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>343</v>
       </c>
@@ -10769,7 +10768,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="308" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>343</v>
       </c>
@@ -10798,7 +10797,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="309" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>343</v>
       </c>
@@ -10827,7 +10826,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="310" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>343</v>
       </c>
@@ -10856,7 +10855,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>345</v>
       </c>
@@ -10885,7 +10884,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>345</v>
       </c>
@@ -10914,7 +10913,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>345</v>
       </c>
@@ -10943,7 +10942,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>345</v>
       </c>
@@ -10972,7 +10971,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>345</v>
       </c>
@@ -11001,7 +11000,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>345</v>
       </c>
@@ -11030,7 +11029,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>345</v>
       </c>
@@ -11059,7 +11058,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>345</v>
       </c>
@@ -11088,7 +11087,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>345</v>
       </c>
@@ -11117,7 +11116,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>356</v>
       </c>
@@ -11146,7 +11145,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="321" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>356</v>
       </c>
@@ -11175,7 +11174,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>359</v>
       </c>
@@ -11204,7 +11203,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="323" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>360</v>
       </c>
@@ -11233,7 +11232,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>360</v>
       </c>
@@ -11262,7 +11261,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>360</v>
       </c>
@@ -11291,7 +11290,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>362</v>
       </c>
@@ -11320,7 +11319,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>363</v>
       </c>
@@ -11349,7 +11348,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>364</v>
       </c>
@@ -11378,7 +11377,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>367</v>
       </c>
@@ -11407,7 +11406,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>367</v>
       </c>
@@ -11436,7 +11435,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>367</v>
       </c>
@@ -11465,7 +11464,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>367</v>
       </c>
@@ -11494,7 +11493,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>369</v>
       </c>
@@ -11523,7 +11522,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="334" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>369</v>
       </c>
@@ -11552,7 +11551,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="335" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>369</v>
       </c>
@@ -11581,7 +11580,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="336" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>369</v>
       </c>
@@ -11610,7 +11609,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="337" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>369</v>
       </c>
@@ -11639,7 +11638,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="338" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>369</v>
       </c>
@@ -11668,7 +11667,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>369</v>
       </c>
@@ -11697,7 +11696,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>372</v>
       </c>
@@ -11726,7 +11725,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>372</v>
       </c>
@@ -11755,7 +11754,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>372</v>
       </c>
@@ -11784,7 +11783,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>372</v>
       </c>
@@ -11813,7 +11812,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>376</v>
       </c>
@@ -11842,7 +11841,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>377</v>
       </c>
@@ -11871,7 +11870,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>377</v>
       </c>
@@ -11900,7 +11899,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="347" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>377</v>
       </c>
@@ -11929,7 +11928,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>377</v>
       </c>
@@ -11958,7 +11957,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="349" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>377</v>
       </c>
@@ -11987,7 +11986,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>379</v>
       </c>
@@ -12016,7 +12015,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="351" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>380</v>
       </c>
@@ -12045,7 +12044,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="352" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>380</v>
       </c>
@@ -12074,7 +12073,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="353" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>380</v>
       </c>
@@ -12103,7 +12102,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="354" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>380</v>
       </c>
@@ -12132,7 +12131,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="355" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>384</v>
       </c>
@@ -12161,7 +12160,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="356" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>385</v>
       </c>
@@ -12190,7 +12189,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="357" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>385</v>
       </c>
@@ -12219,7 +12218,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="358" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>388</v>
       </c>
@@ -12248,7 +12247,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="359" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>390</v>
       </c>
@@ -12277,7 +12276,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="360" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>390</v>
       </c>
@@ -12306,7 +12305,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="361" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>391</v>
       </c>
@@ -12335,7 +12334,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="362" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>391</v>
       </c>
@@ -12364,7 +12363,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="363" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>391</v>
       </c>
@@ -12393,7 +12392,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="364" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>391</v>
       </c>
@@ -12422,7 +12421,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="365" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>391</v>
       </c>
@@ -12451,7 +12450,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="366" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>391</v>
       </c>
@@ -12480,7 +12479,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="367" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>391</v>
       </c>
@@ -12509,7 +12508,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="368" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>391</v>
       </c>
@@ -12538,7 +12537,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="369" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>391</v>
       </c>
@@ -12567,7 +12566,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="370" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>391</v>
       </c>
@@ -12596,7 +12595,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="371" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>391</v>
       </c>
@@ -12625,7 +12624,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="372" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>400</v>
       </c>
@@ -12654,7 +12653,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="373" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>401</v>
       </c>
@@ -12683,7 +12682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="374" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>404</v>
       </c>
@@ -12712,7 +12711,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="375" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>406</v>
       </c>
@@ -12741,7 +12740,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="376" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>406</v>
       </c>
@@ -12770,7 +12769,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="377" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>407</v>
       </c>
@@ -12799,7 +12798,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="378" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>408</v>
       </c>
@@ -12828,7 +12827,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="379" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>408</v>
       </c>
@@ -12857,7 +12856,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="380" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>408</v>
       </c>
@@ -12886,7 +12885,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="381" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>408</v>
       </c>
@@ -12915,7 +12914,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="382" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>408</v>
       </c>
@@ -12944,7 +12943,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="383" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>408</v>
       </c>
@@ -12973,7 +12972,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="384" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>408</v>
       </c>
@@ -13002,7 +13001,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>408</v>
       </c>
@@ -13031,7 +13030,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>408</v>
       </c>
@@ -13060,7 +13059,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>408</v>
       </c>
@@ -13089,7 +13088,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="388" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>416</v>
       </c>
@@ -13118,7 +13117,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="389" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>417</v>
       </c>
@@ -13147,7 +13146,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="390" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>417</v>
       </c>
@@ -13176,7 +13175,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="391" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>418</v>
       </c>
@@ -13205,7 +13204,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>418</v>
       </c>
@@ -13234,7 +13233,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>421</v>
       </c>
@@ -13263,7 +13262,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="394" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>422</v>
       </c>
@@ -13292,7 +13291,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="395" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>422</v>
       </c>
@@ -13321,7 +13320,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="396" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>425</v>
       </c>
@@ -13350,7 +13349,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="397" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>426</v>
       </c>
@@ -13379,7 +13378,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="398" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>426</v>
       </c>
@@ -13408,7 +13407,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="399" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>426</v>
       </c>
@@ -13437,7 +13436,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="400" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>428</v>
       </c>
@@ -13466,7 +13465,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="401" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>431</v>
       </c>
@@ -13495,7 +13494,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="402" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>433</v>
       </c>
@@ -13524,7 +13523,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="403" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>434</v>
       </c>
@@ -13553,7 +13552,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="404" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>434</v>
       </c>
@@ -13582,7 +13581,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>438</v>
       </c>
@@ -13611,7 +13610,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>438</v>
       </c>
@@ -13640,7 +13639,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>438</v>
       </c>
@@ -13669,7 +13668,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="408" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>438</v>
       </c>
@@ -13698,7 +13697,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="409" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>438</v>
       </c>
@@ -13727,7 +13726,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="410" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>440</v>
       </c>
@@ -13756,7 +13755,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="411" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>440</v>
       </c>
@@ -13785,7 +13784,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>440</v>
       </c>
@@ -13814,7 +13813,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="413" spans="1:9" ht="280.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>440</v>
       </c>
@@ -13843,7 +13842,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>440</v>
       </c>
@@ -13872,7 +13871,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="415" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>440</v>
       </c>
@@ -13901,7 +13900,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="416" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>440</v>
       </c>
@@ -13930,7 +13929,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>445</v>
       </c>
@@ -13959,7 +13958,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>446</v>
       </c>
@@ -13988,7 +13987,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="419" spans="1:9" ht="280.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>446</v>
       </c>
@@ -14017,7 +14016,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>446</v>
       </c>
@@ -14046,7 +14045,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="421" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>446</v>
       </c>
@@ -14075,7 +14074,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="422" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>448</v>
       </c>
@@ -14104,7 +14103,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="423" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>449</v>
       </c>
@@ -14133,7 +14132,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="424" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>449</v>
       </c>
@@ -14162,7 +14161,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>449</v>
       </c>
@@ -14191,7 +14190,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>449</v>
       </c>
@@ -14220,7 +14219,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="427" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>449</v>
       </c>
@@ -14249,7 +14248,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="428" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>452</v>
       </c>
@@ -14278,7 +14277,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="429" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>452</v>
       </c>
@@ -14307,7 +14306,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="430" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>453</v>
       </c>
@@ -14336,7 +14335,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="431" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>453</v>
       </c>
@@ -14365,7 +14364,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>453</v>
       </c>
@@ -14394,7 +14393,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="433" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>453</v>
       </c>
@@ -14423,7 +14422,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="434" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>453</v>
       </c>
@@ -14452,7 +14451,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="435" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>453</v>
       </c>
@@ -14481,7 +14480,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="436" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>453</v>
       </c>
@@ -14510,7 +14509,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="437" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>458</v>
       </c>
@@ -14539,7 +14538,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="438" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>458</v>
       </c>
@@ -14568,7 +14567,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="439" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>458</v>
       </c>
@@ -14597,7 +14596,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>458</v>
       </c>
@@ -14626,7 +14625,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="441" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>458</v>
       </c>
@@ -14655,7 +14654,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>458</v>
       </c>
@@ -14684,7 +14683,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="443" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>461</v>
       </c>
@@ -14713,7 +14712,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="444" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>462</v>
       </c>
@@ -14742,7 +14741,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="445" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>462</v>
       </c>
@@ -14771,7 +14770,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="446" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>462</v>
       </c>
@@ -14800,7 +14799,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="447" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>464</v>
       </c>
@@ -14829,7 +14828,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="448" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>464</v>
       </c>
@@ -14858,7 +14857,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="449" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>465</v>
       </c>
@@ -14887,7 +14886,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="450" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>465</v>
       </c>
@@ -14916,7 +14915,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="451" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>466</v>
       </c>
@@ -14945,7 +14944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="452" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>467</v>
       </c>
@@ -14974,20 +14973,14 @@
         <v>69</v>
       </c>
     </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F454" s="3"/>
       <c r="G454" s="3" t="s">
         <v>470</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I452" xr:uid="{2980D243-12F6-47ED-9CB5-E7C7CE140448}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Cuestionario"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I452" xr:uid="{2980D243-12F6-47ED-9CB5-E7C7CE140448}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>